<commit_message>
Update ID randomization to remove duplicate IDs
</commit_message>
<xml_diff>
--- a/ValidationAnalysis/SparseLandmarkingManualAndAutomaticv20180226LOO.xlsx
+++ b/ValidationAnalysis/SparseLandmarkingManualAndAutomaticv20180226LOO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julie White\Box\MyFiles\MyResearch\MeshMonkValidation\ValidationAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{BD64BDFB-AAE2-4C79-A6BB-535354702045}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{227A29E1-83A1-4B92-B95A-31B52C1BF0E5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51120" windowHeight="26740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Combined" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Combined!$A$1:$U$780</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1597" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1597" uniqueCount="99">
   <si>
     <t>ID</t>
   </si>
@@ -204,109 +204,127 @@
     <t>B_ml_x3</t>
   </si>
   <si>
-    <t>MM_124</t>
+    <t>MM_657</t>
   </si>
   <si>
-    <t>MM_172</t>
+    <t>MM_886</t>
   </si>
   <si>
-    <t>MM_130</t>
+    <t>MM_758</t>
   </si>
   <si>
-    <t>MM_154</t>
+    <t>MM_678</t>
   </si>
   <si>
-    <t>MM_156</t>
+    <t>MM_667</t>
   </si>
   <si>
-    <t>MM_143</t>
+    <t>MM_533</t>
   </si>
   <si>
-    <t>MM_137</t>
+    <t>MM_118</t>
+  </si>
+  <si>
+    <t>MM_593</t>
+  </si>
+  <si>
+    <t>MM_582</t>
+  </si>
+  <si>
+    <t>MM_555</t>
+  </si>
+  <si>
+    <t>MM_837</t>
+  </si>
+  <si>
+    <t>MM_515</t>
+  </si>
+  <si>
+    <t>MM_204</t>
+  </si>
+  <si>
+    <t>MM_274</t>
+  </si>
+  <si>
+    <t>MM_623</t>
+  </si>
+  <si>
+    <t>MM_142</t>
+  </si>
+  <si>
+    <t>MM_421</t>
+  </si>
+  <si>
+    <t>MM_163</t>
+  </si>
+  <si>
+    <t>MM_630</t>
+  </si>
+  <si>
+    <t>MM_415</t>
+  </si>
+  <si>
+    <t>MM_747</t>
+  </si>
+  <si>
+    <t>MM_957</t>
+  </si>
+  <si>
+    <t>MM_716</t>
+  </si>
+  <si>
+    <t>MM_978</t>
+  </si>
+  <si>
+    <t>MM_458</t>
+  </si>
+  <si>
+    <t>MM_813</t>
+  </si>
+  <si>
+    <t>MM_588</t>
+  </si>
+  <si>
+    <t>MM_282</t>
+  </si>
+  <si>
+    <t>MM_536</t>
+  </si>
+  <si>
+    <t>MM_559</t>
+  </si>
+  <si>
+    <t>MM_713</t>
+  </si>
+  <si>
+    <t>MM_674</t>
+  </si>
+  <si>
+    <t>MM_770</t>
   </si>
   <si>
     <t>MM_150</t>
   </si>
   <si>
-    <t>MM_153</t>
-  </si>
-  <si>
-    <t>MM_179</t>
-  </si>
-  <si>
-    <t>MM_188</t>
-  </si>
-  <si>
-    <t>MM_142</t>
-  </si>
-  <si>
-    <t>MM_155</t>
-  </si>
-  <si>
-    <t>MM_125</t>
-  </si>
-  <si>
-    <t>MM_175</t>
-  </si>
-  <si>
-    <t>MM_165</t>
-  </si>
-  <si>
     <t>MM_147</t>
   </si>
   <si>
-    <t>MM_102</t>
+    <t>MM_425</t>
   </si>
   <si>
-    <t>MM_189</t>
+    <t>MM_537</t>
   </si>
   <si>
-    <t>MM_148</t>
+    <t>MM_226</t>
   </si>
   <si>
-    <t>MM_170</t>
+    <t>MM_968</t>
   </si>
   <si>
-    <t>MM_157</t>
+    <t>MM_561</t>
   </si>
   <si>
-    <t>MM_177</t>
-  </si>
-  <si>
-    <t>MM_138</t>
-  </si>
-  <si>
-    <t>MM_182</t>
-  </si>
-  <si>
-    <t>MM_120</t>
-  </si>
-  <si>
-    <t>MM_173</t>
-  </si>
-  <si>
-    <t>MM_186</t>
-  </si>
-  <si>
-    <t>MM_132</t>
-  </si>
-  <si>
-    <t>MM_174</t>
-  </si>
-  <si>
-    <t>MM_200</t>
-  </si>
-  <si>
-    <t>MM_160</t>
-  </si>
-  <si>
-    <t>MM_193</t>
-  </si>
-  <si>
-    <t>MM_171</t>
-  </si>
-  <si>
-    <t>MM_141</t>
+    <t>MM_975</t>
   </si>
 </sst>
 </file>
@@ -628,12 +646,12 @@
   <dimension ref="A1:AM780"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.54296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.1796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.08984375" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="8.1796875" bestFit="1" customWidth="1"/>
@@ -32426,7 +32444,7 @@
     </row>
     <row r="268" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A268" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B268">
         <v>1</v>
@@ -32545,7 +32563,7 @@
     </row>
     <row r="269" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A269" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B269">
         <v>2</v>
@@ -32664,7 +32682,7 @@
     </row>
     <row r="270" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A270" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B270">
         <v>3</v>
@@ -32783,7 +32801,7 @@
     </row>
     <row r="271" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A271" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B271">
         <v>4</v>
@@ -32902,7 +32920,7 @@
     </row>
     <row r="272" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A272" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B272">
         <v>5</v>
@@ -33021,7 +33039,7 @@
     </row>
     <row r="273" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A273" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B273">
         <v>6</v>
@@ -33140,7 +33158,7 @@
     </row>
     <row r="274" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A274" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B274">
         <v>7</v>
@@ -33259,7 +33277,7 @@
     </row>
     <row r="275" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A275" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B275">
         <v>8</v>
@@ -33378,7 +33396,7 @@
     </row>
     <row r="276" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A276" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B276">
         <v>9</v>
@@ -33497,7 +33515,7 @@
     </row>
     <row r="277" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A277" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B277">
         <v>10</v>
@@ -33616,7 +33634,7 @@
     </row>
     <row r="278" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A278" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B278">
         <v>11</v>
@@ -33735,7 +33753,7 @@
     </row>
     <row r="279" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A279" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B279">
         <v>12</v>
@@ -33854,7 +33872,7 @@
     </row>
     <row r="280" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A280" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B280">
         <v>13</v>
@@ -33973,7 +33991,7 @@
     </row>
     <row r="281" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A281" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B281">
         <v>14</v>
@@ -34092,7 +34110,7 @@
     </row>
     <row r="282" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A282" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B282">
         <v>15</v>
@@ -34211,7 +34229,7 @@
     </row>
     <row r="283" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A283" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B283">
         <v>16</v>
@@ -34330,7 +34348,7 @@
     </row>
     <row r="284" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A284" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B284">
         <v>17</v>
@@ -34449,7 +34467,7 @@
     </row>
     <row r="285" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A285" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B285">
         <v>18</v>
@@ -34568,7 +34586,7 @@
     </row>
     <row r="286" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A286" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B286">
         <v>19</v>
@@ -34687,7 +34705,7 @@
     </row>
     <row r="287" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A287" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B287">
         <v>1</v>
@@ -34806,7 +34824,7 @@
     </row>
     <row r="288" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A288" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B288">
         <v>2</v>
@@ -34925,7 +34943,7 @@
     </row>
     <row r="289" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A289" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B289">
         <v>3</v>
@@ -35044,7 +35062,7 @@
     </row>
     <row r="290" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A290" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B290">
         <v>4</v>
@@ -35163,7 +35181,7 @@
     </row>
     <row r="291" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A291" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B291">
         <v>5</v>
@@ -35282,7 +35300,7 @@
     </row>
     <row r="292" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A292" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B292">
         <v>6</v>
@@ -35401,7 +35419,7 @@
     </row>
     <row r="293" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A293" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B293">
         <v>7</v>
@@ -35520,7 +35538,7 @@
     </row>
     <row r="294" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A294" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B294">
         <v>8</v>
@@ -35639,7 +35657,7 @@
     </row>
     <row r="295" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A295" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B295">
         <v>9</v>
@@ -35758,7 +35776,7 @@
     </row>
     <row r="296" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A296" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B296">
         <v>10</v>
@@ -35877,7 +35895,7 @@
     </row>
     <row r="297" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A297" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B297">
         <v>11</v>
@@ -35996,7 +36014,7 @@
     </row>
     <row r="298" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A298" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B298">
         <v>12</v>
@@ -36115,7 +36133,7 @@
     </row>
     <row r="299" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A299" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B299">
         <v>13</v>
@@ -36234,7 +36252,7 @@
     </row>
     <row r="300" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A300" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B300">
         <v>14</v>
@@ -36353,7 +36371,7 @@
     </row>
     <row r="301" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A301" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B301">
         <v>15</v>
@@ -36472,7 +36490,7 @@
     </row>
     <row r="302" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A302" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B302">
         <v>16</v>
@@ -36591,7 +36609,7 @@
     </row>
     <row r="303" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A303" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B303">
         <v>17</v>
@@ -36710,7 +36728,7 @@
     </row>
     <row r="304" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A304" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B304">
         <v>18</v>
@@ -36829,7 +36847,7 @@
     </row>
     <row r="305" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A305" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B305">
         <v>19</v>
@@ -36948,7 +36966,7 @@
     </row>
     <row r="306" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A306" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="B306">
         <v>1</v>
@@ -37067,7 +37085,7 @@
     </row>
     <row r="307" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A307" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="B307">
         <v>2</v>
@@ -37186,7 +37204,7 @@
     </row>
     <row r="308" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A308" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="B308">
         <v>3</v>
@@ -37305,7 +37323,7 @@
     </row>
     <row r="309" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A309" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="B309">
         <v>4</v>
@@ -37424,7 +37442,7 @@
     </row>
     <row r="310" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A310" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="B310">
         <v>5</v>
@@ -37543,7 +37561,7 @@
     </row>
     <row r="311" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A311" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="B311">
         <v>6</v>
@@ -37662,7 +37680,7 @@
     </row>
     <row r="312" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A312" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="B312">
         <v>7</v>
@@ -37781,7 +37799,7 @@
     </row>
     <row r="313" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A313" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="B313">
         <v>8</v>
@@ -37900,7 +37918,7 @@
     </row>
     <row r="314" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A314" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="B314">
         <v>9</v>
@@ -38019,7 +38037,7 @@
     </row>
     <row r="315" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A315" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="B315">
         <v>10</v>
@@ -38138,7 +38156,7 @@
     </row>
     <row r="316" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A316" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="B316">
         <v>11</v>
@@ -38257,7 +38275,7 @@
     </row>
     <row r="317" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A317" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="B317">
         <v>12</v>
@@ -38376,7 +38394,7 @@
     </row>
     <row r="318" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A318" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="B318">
         <v>13</v>
@@ -38495,7 +38513,7 @@
     </row>
     <row r="319" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A319" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="B319">
         <v>14</v>
@@ -38614,7 +38632,7 @@
     </row>
     <row r="320" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A320" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="B320">
         <v>15</v>
@@ -38733,7 +38751,7 @@
     </row>
     <row r="321" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A321" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="B321">
         <v>16</v>
@@ -38852,7 +38870,7 @@
     </row>
     <row r="322" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A322" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="B322">
         <v>17</v>
@@ -38971,7 +38989,7 @@
     </row>
     <row r="323" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A323" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="B323">
         <v>18</v>
@@ -39090,7 +39108,7 @@
     </row>
     <row r="324" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A324" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="B324">
         <v>19</v>
@@ -39209,7 +39227,7 @@
     </row>
     <row r="325" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A325" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B325">
         <v>1</v>
@@ -39328,7 +39346,7 @@
     </row>
     <row r="326" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A326" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B326">
         <v>2</v>
@@ -39447,7 +39465,7 @@
     </row>
     <row r="327" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A327" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B327">
         <v>3</v>
@@ -39566,7 +39584,7 @@
     </row>
     <row r="328" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A328" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B328">
         <v>4</v>
@@ -39685,7 +39703,7 @@
     </row>
     <row r="329" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A329" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B329">
         <v>5</v>
@@ -39804,7 +39822,7 @@
     </row>
     <row r="330" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A330" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B330">
         <v>6</v>
@@ -39923,7 +39941,7 @@
     </row>
     <row r="331" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A331" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B331">
         <v>7</v>
@@ -40042,7 +40060,7 @@
     </row>
     <row r="332" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A332" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B332">
         <v>8</v>
@@ -40161,7 +40179,7 @@
     </row>
     <row r="333" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A333" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B333">
         <v>9</v>
@@ -40280,7 +40298,7 @@
     </row>
     <row r="334" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A334" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B334">
         <v>10</v>
@@ -40399,7 +40417,7 @@
     </row>
     <row r="335" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A335" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B335">
         <v>11</v>
@@ -40518,7 +40536,7 @@
     </row>
     <row r="336" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A336" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B336">
         <v>12</v>
@@ -40637,7 +40655,7 @@
     </row>
     <row r="337" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A337" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B337">
         <v>13</v>
@@ -40756,7 +40774,7 @@
     </row>
     <row r="338" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A338" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B338">
         <v>14</v>
@@ -40875,7 +40893,7 @@
     </row>
     <row r="339" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A339" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B339">
         <v>15</v>
@@ -40994,7 +41012,7 @@
     </row>
     <row r="340" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A340" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B340">
         <v>16</v>
@@ -41113,7 +41131,7 @@
     </row>
     <row r="341" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A341" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B341">
         <v>17</v>
@@ -41232,7 +41250,7 @@
     </row>
     <row r="342" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A342" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B342">
         <v>18</v>
@@ -41351,7 +41369,7 @@
     </row>
     <row r="343" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A343" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B343">
         <v>19</v>
@@ -41470,7 +41488,7 @@
     </row>
     <row r="344" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A344" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B344">
         <v>1</v>
@@ -41589,7 +41607,7 @@
     </row>
     <row r="345" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A345" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B345">
         <v>2</v>
@@ -41708,7 +41726,7 @@
     </row>
     <row r="346" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A346" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B346">
         <v>3</v>
@@ -41827,7 +41845,7 @@
     </row>
     <row r="347" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A347" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B347">
         <v>4</v>
@@ -41946,7 +41964,7 @@
     </row>
     <row r="348" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A348" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B348">
         <v>5</v>
@@ -42065,7 +42083,7 @@
     </row>
     <row r="349" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A349" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B349">
         <v>6</v>
@@ -42184,7 +42202,7 @@
     </row>
     <row r="350" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A350" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B350">
         <v>7</v>
@@ -42303,7 +42321,7 @@
     </row>
     <row r="351" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A351" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B351">
         <v>8</v>
@@ -42422,7 +42440,7 @@
     </row>
     <row r="352" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A352" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B352">
         <v>9</v>
@@ -42541,7 +42559,7 @@
     </row>
     <row r="353" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A353" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B353">
         <v>10</v>
@@ -42660,7 +42678,7 @@
     </row>
     <row r="354" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A354" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B354">
         <v>11</v>
@@ -42779,7 +42797,7 @@
     </row>
     <row r="355" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A355" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B355">
         <v>12</v>
@@ -42898,7 +42916,7 @@
     </row>
     <row r="356" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A356" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B356">
         <v>13</v>
@@ -43017,7 +43035,7 @@
     </row>
     <row r="357" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A357" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B357">
         <v>14</v>
@@ -43136,7 +43154,7 @@
     </row>
     <row r="358" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A358" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B358">
         <v>15</v>
@@ -43255,7 +43273,7 @@
     </row>
     <row r="359" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A359" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B359">
         <v>16</v>
@@ -43374,7 +43392,7 @@
     </row>
     <row r="360" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A360" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B360">
         <v>17</v>
@@ -43493,7 +43511,7 @@
     </row>
     <row r="361" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A361" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B361">
         <v>18</v>
@@ -43612,7 +43630,7 @@
     </row>
     <row r="362" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A362" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B362">
         <v>19</v>
@@ -43731,7 +43749,7 @@
     </row>
     <row r="363" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A363" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B363">
         <v>1</v>
@@ -43850,7 +43868,7 @@
     </row>
     <row r="364" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A364" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B364">
         <v>2</v>
@@ -43969,7 +43987,7 @@
     </row>
     <row r="365" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A365" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B365">
         <v>3</v>
@@ -44088,7 +44106,7 @@
     </row>
     <row r="366" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A366" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B366">
         <v>4</v>
@@ -44207,7 +44225,7 @@
     </row>
     <row r="367" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A367" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B367">
         <v>5</v>
@@ -44326,7 +44344,7 @@
     </row>
     <row r="368" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A368" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B368">
         <v>6</v>
@@ -44445,7 +44463,7 @@
     </row>
     <row r="369" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A369" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B369">
         <v>7</v>
@@ -44564,7 +44582,7 @@
     </row>
     <row r="370" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A370" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B370">
         <v>8</v>
@@ -44683,7 +44701,7 @@
     </row>
     <row r="371" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A371" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B371">
         <v>9</v>
@@ -44802,7 +44820,7 @@
     </row>
     <row r="372" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A372" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B372">
         <v>10</v>
@@ -44921,7 +44939,7 @@
     </row>
     <row r="373" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A373" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B373">
         <v>11</v>
@@ -45040,7 +45058,7 @@
     </row>
     <row r="374" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A374" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B374">
         <v>12</v>
@@ -45159,7 +45177,7 @@
     </row>
     <row r="375" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A375" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B375">
         <v>13</v>
@@ -45278,7 +45296,7 @@
     </row>
     <row r="376" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A376" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B376">
         <v>14</v>
@@ -45397,7 +45415,7 @@
     </row>
     <row r="377" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A377" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B377">
         <v>15</v>
@@ -45516,7 +45534,7 @@
     </row>
     <row r="378" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A378" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B378">
         <v>16</v>
@@ -45635,7 +45653,7 @@
     </row>
     <row r="379" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A379" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B379">
         <v>17</v>
@@ -45754,7 +45772,7 @@
     </row>
     <row r="380" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A380" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B380">
         <v>18</v>
@@ -45873,7 +45891,7 @@
     </row>
     <row r="381" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A381" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B381">
         <v>19</v>
@@ -45992,7 +46010,7 @@
     </row>
     <row r="382" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A382" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B382">
         <v>1</v>
@@ -46111,7 +46129,7 @@
     </row>
     <row r="383" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A383" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B383">
         <v>2</v>
@@ -46230,7 +46248,7 @@
     </row>
     <row r="384" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A384" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B384">
         <v>3</v>
@@ -46349,7 +46367,7 @@
     </row>
     <row r="385" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A385" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B385">
         <v>4</v>
@@ -46468,7 +46486,7 @@
     </row>
     <row r="386" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A386" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B386">
         <v>5</v>
@@ -46587,7 +46605,7 @@
     </row>
     <row r="387" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A387" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B387">
         <v>6</v>
@@ -46706,7 +46724,7 @@
     </row>
     <row r="388" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A388" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B388">
         <v>7</v>
@@ -46825,7 +46843,7 @@
     </row>
     <row r="389" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A389" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B389">
         <v>8</v>
@@ -46944,7 +46962,7 @@
     </row>
     <row r="390" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A390" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B390">
         <v>9</v>
@@ -47063,7 +47081,7 @@
     </row>
     <row r="391" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A391" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B391">
         <v>10</v>
@@ -47182,7 +47200,7 @@
     </row>
     <row r="392" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A392" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B392">
         <v>11</v>
@@ -47301,7 +47319,7 @@
     </row>
     <row r="393" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A393" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B393">
         <v>12</v>
@@ -47420,7 +47438,7 @@
     </row>
     <row r="394" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A394" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B394">
         <v>13</v>
@@ -47539,7 +47557,7 @@
     </row>
     <row r="395" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A395" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B395">
         <v>14</v>
@@ -47658,7 +47676,7 @@
     </row>
     <row r="396" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A396" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B396">
         <v>15</v>
@@ -47777,7 +47795,7 @@
     </row>
     <row r="397" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A397" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B397">
         <v>16</v>
@@ -47896,7 +47914,7 @@
     </row>
     <row r="398" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A398" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B398">
         <v>17</v>
@@ -48015,7 +48033,7 @@
     </row>
     <row r="399" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A399" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B399">
         <v>18</v>
@@ -48134,7 +48152,7 @@
     </row>
     <row r="400" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A400" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B400">
         <v>19</v>
@@ -48253,7 +48271,7 @@
     </row>
     <row r="401" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A401" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="B401">
         <v>1</v>
@@ -48372,7 +48390,7 @@
     </row>
     <row r="402" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A402" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="B402">
         <v>2</v>
@@ -48491,7 +48509,7 @@
     </row>
     <row r="403" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A403" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="B403">
         <v>3</v>
@@ -48610,7 +48628,7 @@
     </row>
     <row r="404" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A404" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="B404">
         <v>4</v>
@@ -48729,7 +48747,7 @@
     </row>
     <row r="405" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A405" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="B405">
         <v>5</v>
@@ -48848,7 +48866,7 @@
     </row>
     <row r="406" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A406" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="B406">
         <v>6</v>
@@ -48967,7 +48985,7 @@
     </row>
     <row r="407" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A407" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="B407">
         <v>7</v>
@@ -49086,7 +49104,7 @@
     </row>
     <row r="408" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A408" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="B408">
         <v>8</v>
@@ -49205,7 +49223,7 @@
     </row>
     <row r="409" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A409" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="B409">
         <v>9</v>
@@ -49324,7 +49342,7 @@
     </row>
     <row r="410" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A410" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="B410">
         <v>10</v>
@@ -49443,7 +49461,7 @@
     </row>
     <row r="411" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A411" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="B411">
         <v>11</v>
@@ -49562,7 +49580,7 @@
     </row>
     <row r="412" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A412" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="B412">
         <v>12</v>
@@ -49681,7 +49699,7 @@
     </row>
     <row r="413" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A413" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="B413">
         <v>13</v>
@@ -49800,7 +49818,7 @@
     </row>
     <row r="414" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A414" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="B414">
         <v>14</v>
@@ -49919,7 +49937,7 @@
     </row>
     <row r="415" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A415" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="B415">
         <v>15</v>
@@ -50038,7 +50056,7 @@
     </row>
     <row r="416" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A416" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="B416">
         <v>16</v>
@@ -50157,7 +50175,7 @@
     </row>
     <row r="417" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A417" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="B417">
         <v>17</v>
@@ -50276,7 +50294,7 @@
     </row>
     <row r="418" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A418" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="B418">
         <v>18</v>
@@ -50395,7 +50413,7 @@
     </row>
     <row r="419" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A419" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="B419">
         <v>19</v>
@@ -50514,7 +50532,7 @@
     </row>
     <row r="420" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A420" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B420">
         <v>1</v>
@@ -50633,7 +50651,7 @@
     </row>
     <row r="421" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A421" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B421">
         <v>2</v>
@@ -50752,7 +50770,7 @@
     </row>
     <row r="422" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A422" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B422">
         <v>3</v>
@@ -50871,7 +50889,7 @@
     </row>
     <row r="423" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A423" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B423">
         <v>4</v>
@@ -50990,7 +51008,7 @@
     </row>
     <row r="424" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A424" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B424">
         <v>5</v>
@@ -51109,7 +51127,7 @@
     </row>
     <row r="425" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A425" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B425">
         <v>6</v>
@@ -51228,7 +51246,7 @@
     </row>
     <row r="426" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A426" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B426">
         <v>7</v>
@@ -51347,7 +51365,7 @@
     </row>
     <row r="427" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A427" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B427">
         <v>8</v>
@@ -51466,7 +51484,7 @@
     </row>
     <row r="428" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A428" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B428">
         <v>9</v>
@@ -51585,7 +51603,7 @@
     </row>
     <row r="429" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A429" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B429">
         <v>10</v>
@@ -51704,7 +51722,7 @@
     </row>
     <row r="430" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A430" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B430">
         <v>11</v>
@@ -51823,7 +51841,7 @@
     </row>
     <row r="431" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A431" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B431">
         <v>12</v>
@@ -51942,7 +51960,7 @@
     </row>
     <row r="432" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A432" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B432">
         <v>13</v>
@@ -52061,7 +52079,7 @@
     </row>
     <row r="433" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A433" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B433">
         <v>14</v>
@@ -52180,7 +52198,7 @@
     </row>
     <row r="434" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A434" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B434">
         <v>15</v>
@@ -52299,7 +52317,7 @@
     </row>
     <row r="435" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A435" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B435">
         <v>16</v>
@@ -52418,7 +52436,7 @@
     </row>
     <row r="436" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A436" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B436">
         <v>17</v>
@@ -52537,7 +52555,7 @@
     </row>
     <row r="437" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A437" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B437">
         <v>18</v>
@@ -52656,7 +52674,7 @@
     </row>
     <row r="438" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A438" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B438">
         <v>19</v>
@@ -52775,7 +52793,7 @@
     </row>
     <row r="439" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A439" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="B439">
         <v>1</v>
@@ -52894,7 +52912,7 @@
     </row>
     <row r="440" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A440" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="B440">
         <v>2</v>
@@ -53013,7 +53031,7 @@
     </row>
     <row r="441" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A441" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="B441">
         <v>3</v>
@@ -53132,7 +53150,7 @@
     </row>
     <row r="442" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A442" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="B442">
         <v>4</v>
@@ -53251,7 +53269,7 @@
     </row>
     <row r="443" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A443" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="B443">
         <v>5</v>
@@ -53370,7 +53388,7 @@
     </row>
     <row r="444" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A444" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="B444">
         <v>6</v>
@@ -53489,7 +53507,7 @@
     </row>
     <row r="445" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A445" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="B445">
         <v>7</v>
@@ -53608,7 +53626,7 @@
     </row>
     <row r="446" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A446" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="B446">
         <v>8</v>
@@ -53727,7 +53745,7 @@
     </row>
     <row r="447" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A447" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="B447">
         <v>9</v>
@@ -53846,7 +53864,7 @@
     </row>
     <row r="448" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A448" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="B448">
         <v>10</v>
@@ -53965,7 +53983,7 @@
     </row>
     <row r="449" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A449" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="B449">
         <v>11</v>
@@ -54084,7 +54102,7 @@
     </row>
     <row r="450" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A450" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="B450">
         <v>12</v>
@@ -54203,7 +54221,7 @@
     </row>
     <row r="451" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A451" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="B451">
         <v>13</v>
@@ -54322,7 +54340,7 @@
     </row>
     <row r="452" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A452" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="B452">
         <v>14</v>
@@ -54441,7 +54459,7 @@
     </row>
     <row r="453" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A453" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="B453">
         <v>15</v>
@@ -54560,7 +54578,7 @@
     </row>
     <row r="454" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A454" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="B454">
         <v>16</v>
@@ -54679,7 +54697,7 @@
     </row>
     <row r="455" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A455" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="B455">
         <v>17</v>
@@ -54798,7 +54816,7 @@
     </row>
     <row r="456" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A456" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="B456">
         <v>18</v>
@@ -54917,7 +54935,7 @@
     </row>
     <row r="457" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A457" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="B457">
         <v>19</v>
@@ -55036,7 +55054,7 @@
     </row>
     <row r="458" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A458" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="B458">
         <v>1</v>
@@ -55155,7 +55173,7 @@
     </row>
     <row r="459" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A459" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="B459">
         <v>2</v>
@@ -55274,7 +55292,7 @@
     </row>
     <row r="460" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A460" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="B460">
         <v>3</v>
@@ -55393,7 +55411,7 @@
     </row>
     <row r="461" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A461" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="B461">
         <v>4</v>
@@ -55512,7 +55530,7 @@
     </row>
     <row r="462" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A462" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="B462">
         <v>5</v>
@@ -55631,7 +55649,7 @@
     </row>
     <row r="463" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A463" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="B463">
         <v>6</v>
@@ -55750,7 +55768,7 @@
     </row>
     <row r="464" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A464" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="B464">
         <v>7</v>
@@ -55869,7 +55887,7 @@
     </row>
     <row r="465" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A465" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="B465">
         <v>8</v>
@@ -55988,7 +56006,7 @@
     </row>
     <row r="466" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A466" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="B466">
         <v>9</v>
@@ -56107,7 +56125,7 @@
     </row>
     <row r="467" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A467" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="B467">
         <v>10</v>
@@ -56226,7 +56244,7 @@
     </row>
     <row r="468" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A468" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="B468">
         <v>11</v>
@@ -56345,7 +56363,7 @@
     </row>
     <row r="469" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A469" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="B469">
         <v>12</v>
@@ -56464,7 +56482,7 @@
     </row>
     <row r="470" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A470" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="B470">
         <v>13</v>
@@ -56583,7 +56601,7 @@
     </row>
     <row r="471" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A471" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="B471">
         <v>14</v>
@@ -56702,7 +56720,7 @@
     </row>
     <row r="472" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A472" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="B472">
         <v>15</v>
@@ -56821,7 +56839,7 @@
     </row>
     <row r="473" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A473" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="B473">
         <v>16</v>
@@ -56940,7 +56958,7 @@
     </row>
     <row r="474" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A474" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="B474">
         <v>17</v>
@@ -57059,7 +57077,7 @@
     </row>
     <row r="475" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A475" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="B475">
         <v>18</v>
@@ -57178,7 +57196,7 @@
     </row>
     <row r="476" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A476" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="B476">
         <v>19</v>
@@ -57297,7 +57315,7 @@
     </row>
     <row r="477" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A477" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B477">
         <v>1</v>
@@ -57416,7 +57434,7 @@
     </row>
     <row r="478" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A478" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B478">
         <v>2</v>
@@ -57535,7 +57553,7 @@
     </row>
     <row r="479" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A479" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B479">
         <v>3</v>
@@ -57654,7 +57672,7 @@
     </row>
     <row r="480" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A480" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B480">
         <v>4</v>
@@ -57773,7 +57791,7 @@
     </row>
     <row r="481" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A481" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B481">
         <v>5</v>
@@ -57892,7 +57910,7 @@
     </row>
     <row r="482" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A482" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B482">
         <v>6</v>
@@ -58011,7 +58029,7 @@
     </row>
     <row r="483" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A483" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B483">
         <v>7</v>
@@ -58130,7 +58148,7 @@
     </row>
     <row r="484" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A484" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B484">
         <v>8</v>
@@ -58249,7 +58267,7 @@
     </row>
     <row r="485" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A485" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B485">
         <v>9</v>
@@ -58368,7 +58386,7 @@
     </row>
     <row r="486" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A486" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B486">
         <v>10</v>
@@ -58487,7 +58505,7 @@
     </row>
     <row r="487" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A487" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B487">
         <v>11</v>
@@ -58606,7 +58624,7 @@
     </row>
     <row r="488" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A488" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B488">
         <v>12</v>
@@ -58725,7 +58743,7 @@
     </row>
     <row r="489" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A489" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B489">
         <v>13</v>
@@ -58844,7 +58862,7 @@
     </row>
     <row r="490" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A490" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B490">
         <v>14</v>
@@ -58963,7 +58981,7 @@
     </row>
     <row r="491" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A491" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B491">
         <v>15</v>
@@ -59082,7 +59100,7 @@
     </row>
     <row r="492" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A492" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B492">
         <v>16</v>
@@ -59201,7 +59219,7 @@
     </row>
     <row r="493" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A493" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B493">
         <v>17</v>
@@ -59320,7 +59338,7 @@
     </row>
     <row r="494" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A494" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B494">
         <v>18</v>
@@ -59439,7 +59457,7 @@
     </row>
     <row r="495" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A495" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B495">
         <v>19</v>
@@ -59558,7 +59576,7 @@
     </row>
     <row r="496" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A496" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="B496">
         <v>1</v>
@@ -59677,7 +59695,7 @@
     </row>
     <row r="497" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A497" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="B497">
         <v>2</v>
@@ -59796,7 +59814,7 @@
     </row>
     <row r="498" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A498" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="B498">
         <v>3</v>
@@ -59915,7 +59933,7 @@
     </row>
     <row r="499" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A499" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="B499">
         <v>4</v>
@@ -60034,7 +60052,7 @@
     </row>
     <row r="500" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A500" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="B500">
         <v>5</v>
@@ -60153,7 +60171,7 @@
     </row>
     <row r="501" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A501" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="B501">
         <v>6</v>
@@ -60272,7 +60290,7 @@
     </row>
     <row r="502" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A502" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="B502">
         <v>7</v>
@@ -60391,7 +60409,7 @@
     </row>
     <row r="503" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A503" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="B503">
         <v>8</v>
@@ -60510,7 +60528,7 @@
     </row>
     <row r="504" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A504" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="B504">
         <v>9</v>
@@ -60629,7 +60647,7 @@
     </row>
     <row r="505" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A505" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="B505">
         <v>10</v>
@@ -60748,7 +60766,7 @@
     </row>
     <row r="506" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A506" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="B506">
         <v>11</v>
@@ -60867,7 +60885,7 @@
     </row>
     <row r="507" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A507" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="B507">
         <v>12</v>
@@ -60986,7 +61004,7 @@
     </row>
     <row r="508" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A508" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="B508">
         <v>13</v>
@@ -61105,7 +61123,7 @@
     </row>
     <row r="509" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A509" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="B509">
         <v>14</v>
@@ -61224,7 +61242,7 @@
     </row>
     <row r="510" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A510" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="B510">
         <v>15</v>
@@ -61343,7 +61361,7 @@
     </row>
     <row r="511" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A511" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="B511">
         <v>16</v>
@@ -61462,7 +61480,7 @@
     </row>
     <row r="512" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A512" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="B512">
         <v>17</v>
@@ -61581,7 +61599,7 @@
     </row>
     <row r="513" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A513" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="B513">
         <v>18</v>
@@ -61700,7 +61718,7 @@
     </row>
     <row r="514" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A514" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="B514">
         <v>19</v>
@@ -61819,7 +61837,7 @@
     </row>
     <row r="515" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A515" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="B515">
         <v>1</v>
@@ -61938,7 +61956,7 @@
     </row>
     <row r="516" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A516" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="B516">
         <v>2</v>
@@ -62057,7 +62075,7 @@
     </row>
     <row r="517" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A517" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="B517">
         <v>3</v>
@@ -62176,7 +62194,7 @@
     </row>
     <row r="518" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A518" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="B518">
         <v>4</v>
@@ -62295,7 +62313,7 @@
     </row>
     <row r="519" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A519" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="B519">
         <v>5</v>
@@ -62414,7 +62432,7 @@
     </row>
     <row r="520" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A520" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="B520">
         <v>6</v>
@@ -62533,7 +62551,7 @@
     </row>
     <row r="521" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A521" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="B521">
         <v>7</v>
@@ -62652,7 +62670,7 @@
     </row>
     <row r="522" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A522" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="B522">
         <v>8</v>
@@ -62771,7 +62789,7 @@
     </row>
     <row r="523" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A523" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="B523">
         <v>9</v>
@@ -62890,7 +62908,7 @@
     </row>
     <row r="524" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A524" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="B524">
         <v>10</v>
@@ -63009,7 +63027,7 @@
     </row>
     <row r="525" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A525" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="B525">
         <v>11</v>
@@ -63128,7 +63146,7 @@
     </row>
     <row r="526" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A526" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="B526">
         <v>12</v>
@@ -63247,7 +63265,7 @@
     </row>
     <row r="527" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A527" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="B527">
         <v>13</v>
@@ -63366,7 +63384,7 @@
     </row>
     <row r="528" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A528" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="B528">
         <v>14</v>
@@ -63485,7 +63503,7 @@
     </row>
     <row r="529" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A529" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="B529">
         <v>15</v>
@@ -63604,7 +63622,7 @@
     </row>
     <row r="530" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A530" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="B530">
         <v>16</v>
@@ -63723,7 +63741,7 @@
     </row>
     <row r="531" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A531" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="B531">
         <v>17</v>
@@ -63842,7 +63860,7 @@
     </row>
     <row r="532" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A532" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="B532">
         <v>18</v>
@@ -63961,7 +63979,7 @@
     </row>
     <row r="533" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A533" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="B533">
         <v>19</v>
@@ -64080,7 +64098,7 @@
     </row>
     <row r="534" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A534" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="B534">
         <v>1</v>
@@ -64199,7 +64217,7 @@
     </row>
     <row r="535" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A535" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="B535">
         <v>2</v>
@@ -64318,7 +64336,7 @@
     </row>
     <row r="536" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A536" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="B536">
         <v>3</v>
@@ -64437,7 +64455,7 @@
     </row>
     <row r="537" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A537" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="B537">
         <v>4</v>
@@ -64556,7 +64574,7 @@
     </row>
     <row r="538" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A538" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="B538">
         <v>5</v>
@@ -64675,7 +64693,7 @@
     </row>
     <row r="539" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A539" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="B539">
         <v>6</v>
@@ -64794,7 +64812,7 @@
     </row>
     <row r="540" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A540" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="B540">
         <v>7</v>
@@ -64913,7 +64931,7 @@
     </row>
     <row r="541" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A541" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="B541">
         <v>8</v>
@@ -65032,7 +65050,7 @@
     </row>
     <row r="542" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A542" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="B542">
         <v>9</v>
@@ -65151,7 +65169,7 @@
     </row>
     <row r="543" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A543" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="B543">
         <v>10</v>
@@ -65270,7 +65288,7 @@
     </row>
     <row r="544" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A544" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="B544">
         <v>11</v>
@@ -65389,7 +65407,7 @@
     </row>
     <row r="545" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A545" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="B545">
         <v>12</v>
@@ -65508,7 +65526,7 @@
     </row>
     <row r="546" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A546" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="B546">
         <v>13</v>
@@ -65627,7 +65645,7 @@
     </row>
     <row r="547" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A547" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="B547">
         <v>14</v>
@@ -65746,7 +65764,7 @@
     </row>
     <row r="548" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A548" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="B548">
         <v>15</v>
@@ -65865,7 +65883,7 @@
     </row>
     <row r="549" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A549" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="B549">
         <v>16</v>
@@ -65984,7 +66002,7 @@
     </row>
     <row r="550" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A550" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="B550">
         <v>17</v>
@@ -66103,7 +66121,7 @@
     </row>
     <row r="551" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A551" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="B551">
         <v>18</v>
@@ -66222,7 +66240,7 @@
     </row>
     <row r="552" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A552" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="B552">
         <v>19</v>
@@ -66341,7 +66359,7 @@
     </row>
     <row r="553" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A553" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="B553">
         <v>1</v>
@@ -66460,7 +66478,7 @@
     </row>
     <row r="554" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A554" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="B554">
         <v>2</v>
@@ -66579,7 +66597,7 @@
     </row>
     <row r="555" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A555" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="B555">
         <v>3</v>
@@ -66698,7 +66716,7 @@
     </row>
     <row r="556" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A556" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="B556">
         <v>4</v>
@@ -66817,7 +66835,7 @@
     </row>
     <row r="557" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A557" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="B557">
         <v>5</v>
@@ -66936,7 +66954,7 @@
     </row>
     <row r="558" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A558" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="B558">
         <v>6</v>
@@ -67055,7 +67073,7 @@
     </row>
     <row r="559" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A559" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="B559">
         <v>7</v>
@@ -67174,7 +67192,7 @@
     </row>
     <row r="560" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A560" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="B560">
         <v>8</v>
@@ -67293,7 +67311,7 @@
     </row>
     <row r="561" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A561" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="B561">
         <v>9</v>
@@ -67412,7 +67430,7 @@
     </row>
     <row r="562" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A562" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="B562">
         <v>10</v>
@@ -67531,7 +67549,7 @@
     </row>
     <row r="563" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A563" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="B563">
         <v>11</v>
@@ -67650,7 +67668,7 @@
     </row>
     <row r="564" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A564" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="B564">
         <v>12</v>
@@ -67769,7 +67787,7 @@
     </row>
     <row r="565" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A565" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="B565">
         <v>13</v>
@@ -67888,7 +67906,7 @@
     </row>
     <row r="566" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A566" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="B566">
         <v>14</v>
@@ -68007,7 +68025,7 @@
     </row>
     <row r="567" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A567" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="B567">
         <v>15</v>
@@ -68126,7 +68144,7 @@
     </row>
     <row r="568" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A568" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="B568">
         <v>16</v>
@@ -68245,7 +68263,7 @@
     </row>
     <row r="569" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A569" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="B569">
         <v>17</v>
@@ -68364,7 +68382,7 @@
     </row>
     <row r="570" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A570" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="B570">
         <v>18</v>
@@ -68483,7 +68501,7 @@
     </row>
     <row r="571" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A571" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="B571">
         <v>19</v>
@@ -68602,7 +68620,7 @@
     </row>
     <row r="572" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A572" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="B572">
         <v>1</v>
@@ -68721,7 +68739,7 @@
     </row>
     <row r="573" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A573" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="B573">
         <v>2</v>
@@ -68840,7 +68858,7 @@
     </row>
     <row r="574" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A574" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="B574">
         <v>3</v>
@@ -68959,7 +68977,7 @@
     </row>
     <row r="575" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A575" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="B575">
         <v>4</v>
@@ -69078,7 +69096,7 @@
     </row>
     <row r="576" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A576" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="B576">
         <v>5</v>
@@ -69197,7 +69215,7 @@
     </row>
     <row r="577" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A577" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="B577">
         <v>6</v>
@@ -69316,7 +69334,7 @@
     </row>
     <row r="578" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A578" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="B578">
         <v>7</v>
@@ -69435,7 +69453,7 @@
     </row>
     <row r="579" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A579" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="B579">
         <v>8</v>
@@ -69554,7 +69572,7 @@
     </row>
     <row r="580" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A580" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="B580">
         <v>9</v>
@@ -69673,7 +69691,7 @@
     </row>
     <row r="581" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A581" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="B581">
         <v>10</v>
@@ -69792,7 +69810,7 @@
     </row>
     <row r="582" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A582" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="B582">
         <v>11</v>
@@ -69911,7 +69929,7 @@
     </row>
     <row r="583" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A583" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="B583">
         <v>12</v>
@@ -70030,7 +70048,7 @@
     </row>
     <row r="584" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A584" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="B584">
         <v>13</v>
@@ -70149,7 +70167,7 @@
     </row>
     <row r="585" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A585" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="B585">
         <v>14</v>
@@ -70268,7 +70286,7 @@
     </row>
     <row r="586" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A586" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="B586">
         <v>15</v>
@@ -70387,7 +70405,7 @@
     </row>
     <row r="587" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A587" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="B587">
         <v>16</v>
@@ -70506,7 +70524,7 @@
     </row>
     <row r="588" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A588" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="B588">
         <v>17</v>
@@ -70625,7 +70643,7 @@
     </row>
     <row r="589" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A589" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="B589">
         <v>18</v>
@@ -70744,7 +70762,7 @@
     </row>
     <row r="590" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A590" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="B590">
         <v>19</v>
@@ -70863,7 +70881,7 @@
     </row>
     <row r="591" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A591" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="B591">
         <v>1</v>
@@ -70982,7 +71000,7 @@
     </row>
     <row r="592" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A592" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="B592">
         <v>2</v>
@@ -71101,7 +71119,7 @@
     </row>
     <row r="593" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A593" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="B593">
         <v>3</v>
@@ -71220,7 +71238,7 @@
     </row>
     <row r="594" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A594" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="B594">
         <v>4</v>
@@ -71339,7 +71357,7 @@
     </row>
     <row r="595" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A595" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="B595">
         <v>5</v>
@@ -71458,7 +71476,7 @@
     </row>
     <row r="596" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A596" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="B596">
         <v>6</v>
@@ -71577,7 +71595,7 @@
     </row>
     <row r="597" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A597" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="B597">
         <v>7</v>
@@ -71696,7 +71714,7 @@
     </row>
     <row r="598" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A598" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="B598">
         <v>8</v>
@@ -71815,7 +71833,7 @@
     </row>
     <row r="599" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A599" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="B599">
         <v>9</v>
@@ -71934,7 +71952,7 @@
     </row>
     <row r="600" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A600" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="B600">
         <v>10</v>
@@ -72053,7 +72071,7 @@
     </row>
     <row r="601" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A601" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="B601">
         <v>11</v>
@@ -72172,7 +72190,7 @@
     </row>
     <row r="602" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A602" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="B602">
         <v>12</v>
@@ -72291,7 +72309,7 @@
     </row>
     <row r="603" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A603" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="B603">
         <v>13</v>
@@ -72410,7 +72428,7 @@
     </row>
     <row r="604" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A604" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="B604">
         <v>14</v>
@@ -72529,7 +72547,7 @@
     </row>
     <row r="605" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A605" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="B605">
         <v>15</v>
@@ -72648,7 +72666,7 @@
     </row>
     <row r="606" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A606" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="B606">
         <v>16</v>
@@ -72767,7 +72785,7 @@
     </row>
     <row r="607" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A607" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="B607">
         <v>17</v>
@@ -72886,7 +72904,7 @@
     </row>
     <row r="608" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A608" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="B608">
         <v>18</v>
@@ -73005,7 +73023,7 @@
     </row>
     <row r="609" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A609" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="B609">
         <v>19</v>
@@ -73124,7 +73142,7 @@
     </row>
     <row r="610" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A610" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="B610">
         <v>1</v>
@@ -73243,7 +73261,7 @@
     </row>
     <row r="611" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A611" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="B611">
         <v>2</v>
@@ -73362,7 +73380,7 @@
     </row>
     <row r="612" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A612" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="B612">
         <v>3</v>
@@ -73481,7 +73499,7 @@
     </row>
     <row r="613" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A613" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="B613">
         <v>4</v>
@@ -73600,7 +73618,7 @@
     </row>
     <row r="614" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A614" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="B614">
         <v>5</v>
@@ -73719,7 +73737,7 @@
     </row>
     <row r="615" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A615" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="B615">
         <v>6</v>
@@ -73838,7 +73856,7 @@
     </row>
     <row r="616" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A616" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="B616">
         <v>7</v>
@@ -73957,7 +73975,7 @@
     </row>
     <row r="617" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A617" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="B617">
         <v>8</v>
@@ -74076,7 +74094,7 @@
     </row>
     <row r="618" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A618" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="B618">
         <v>9</v>
@@ -74195,7 +74213,7 @@
     </row>
     <row r="619" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A619" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="B619">
         <v>10</v>
@@ -74314,7 +74332,7 @@
     </row>
     <row r="620" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A620" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="B620">
         <v>11</v>
@@ -74433,7 +74451,7 @@
     </row>
     <row r="621" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A621" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="B621">
         <v>12</v>
@@ -74552,7 +74570,7 @@
     </row>
     <row r="622" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A622" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="B622">
         <v>13</v>
@@ -74671,7 +74689,7 @@
     </row>
     <row r="623" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A623" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="B623">
         <v>14</v>
@@ -74790,7 +74808,7 @@
     </row>
     <row r="624" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A624" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="B624">
         <v>15</v>
@@ -74909,7 +74927,7 @@
     </row>
     <row r="625" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A625" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="B625">
         <v>16</v>
@@ -75028,7 +75046,7 @@
     </row>
     <row r="626" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A626" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="B626">
         <v>17</v>
@@ -75147,7 +75165,7 @@
     </row>
     <row r="627" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A627" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="B627">
         <v>18</v>
@@ -75266,7 +75284,7 @@
     </row>
     <row r="628" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A628" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="B628">
         <v>19</v>
@@ -75385,7 +75403,7 @@
     </row>
     <row r="629" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A629" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="B629">
         <v>1</v>
@@ -75504,7 +75522,7 @@
     </row>
     <row r="630" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A630" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="B630">
         <v>2</v>
@@ -75623,7 +75641,7 @@
     </row>
     <row r="631" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A631" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="B631">
         <v>3</v>
@@ -75742,7 +75760,7 @@
     </row>
     <row r="632" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A632" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="B632">
         <v>4</v>
@@ -75861,7 +75879,7 @@
     </row>
     <row r="633" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A633" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="B633">
         <v>5</v>
@@ -75980,7 +75998,7 @@
     </row>
     <row r="634" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A634" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="B634">
         <v>6</v>
@@ -76099,7 +76117,7 @@
     </row>
     <row r="635" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A635" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="B635">
         <v>7</v>
@@ -76218,7 +76236,7 @@
     </row>
     <row r="636" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A636" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="B636">
         <v>8</v>
@@ -76337,7 +76355,7 @@
     </row>
     <row r="637" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A637" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="B637">
         <v>9</v>
@@ -76456,7 +76474,7 @@
     </row>
     <row r="638" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A638" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="B638">
         <v>10</v>
@@ -76575,7 +76593,7 @@
     </row>
     <row r="639" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A639" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="B639">
         <v>11</v>
@@ -76694,7 +76712,7 @@
     </row>
     <row r="640" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A640" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="B640">
         <v>12</v>
@@ -76813,7 +76831,7 @@
     </row>
     <row r="641" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A641" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="B641">
         <v>13</v>
@@ -76932,7 +76950,7 @@
     </row>
     <row r="642" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A642" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="B642">
         <v>14</v>
@@ -77051,7 +77069,7 @@
     </row>
     <row r="643" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A643" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="B643">
         <v>15</v>
@@ -77170,7 +77188,7 @@
     </row>
     <row r="644" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A644" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="B644">
         <v>16</v>
@@ -77289,7 +77307,7 @@
     </row>
     <row r="645" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A645" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="B645">
         <v>17</v>
@@ -77408,7 +77426,7 @@
     </row>
     <row r="646" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A646" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="B646">
         <v>18</v>
@@ -77527,7 +77545,7 @@
     </row>
     <row r="647" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A647" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="B647">
         <v>19</v>
@@ -77646,7 +77664,7 @@
     </row>
     <row r="648" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A648" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="B648">
         <v>1</v>
@@ -77765,7 +77783,7 @@
     </row>
     <row r="649" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A649" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="B649">
         <v>2</v>
@@ -77884,7 +77902,7 @@
     </row>
     <row r="650" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A650" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="B650">
         <v>3</v>
@@ -78003,7 +78021,7 @@
     </row>
     <row r="651" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A651" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="B651">
         <v>4</v>
@@ -78122,7 +78140,7 @@
     </row>
     <row r="652" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A652" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="B652">
         <v>5</v>
@@ -78241,7 +78259,7 @@
     </row>
     <row r="653" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A653" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="B653">
         <v>6</v>
@@ -78360,7 +78378,7 @@
     </row>
     <row r="654" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A654" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="B654">
         <v>7</v>
@@ -78479,7 +78497,7 @@
     </row>
     <row r="655" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A655" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="B655">
         <v>8</v>
@@ -78598,7 +78616,7 @@
     </row>
     <row r="656" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A656" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="B656">
         <v>9</v>
@@ -78717,7 +78735,7 @@
     </row>
     <row r="657" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A657" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="B657">
         <v>10</v>
@@ -78836,7 +78854,7 @@
     </row>
     <row r="658" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A658" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="B658">
         <v>11</v>
@@ -78955,7 +78973,7 @@
     </row>
     <row r="659" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A659" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="B659">
         <v>12</v>
@@ -79074,7 +79092,7 @@
     </row>
     <row r="660" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A660" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="B660">
         <v>13</v>
@@ -79193,7 +79211,7 @@
     </row>
     <row r="661" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A661" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="B661">
         <v>14</v>
@@ -79312,7 +79330,7 @@
     </row>
     <row r="662" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A662" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="B662">
         <v>15</v>
@@ -79431,7 +79449,7 @@
     </row>
     <row r="663" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A663" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="B663">
         <v>16</v>
@@ -79550,7 +79568,7 @@
     </row>
     <row r="664" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A664" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="B664">
         <v>17</v>
@@ -79669,7 +79687,7 @@
     </row>
     <row r="665" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A665" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="B665">
         <v>18</v>
@@ -79788,7 +79806,7 @@
     </row>
     <row r="666" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A666" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="B666">
         <v>19</v>
@@ -79907,7 +79925,7 @@
     </row>
     <row r="667" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A667" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="B667">
         <v>1</v>
@@ -80026,7 +80044,7 @@
     </row>
     <row r="668" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A668" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="B668">
         <v>2</v>
@@ -80145,7 +80163,7 @@
     </row>
     <row r="669" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A669" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="B669">
         <v>3</v>
@@ -80264,7 +80282,7 @@
     </row>
     <row r="670" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A670" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="B670">
         <v>4</v>
@@ -80383,7 +80401,7 @@
     </row>
     <row r="671" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A671" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="B671">
         <v>5</v>
@@ -80502,7 +80520,7 @@
     </row>
     <row r="672" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A672" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="B672">
         <v>6</v>
@@ -80621,7 +80639,7 @@
     </row>
     <row r="673" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A673" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="B673">
         <v>7</v>
@@ -80740,7 +80758,7 @@
     </row>
     <row r="674" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A674" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="B674">
         <v>8</v>
@@ -80859,7 +80877,7 @@
     </row>
     <row r="675" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A675" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="B675">
         <v>9</v>
@@ -80978,7 +80996,7 @@
     </row>
     <row r="676" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A676" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="B676">
         <v>10</v>
@@ -81097,7 +81115,7 @@
     </row>
     <row r="677" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A677" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="B677">
         <v>11</v>
@@ -81216,7 +81234,7 @@
     </row>
     <row r="678" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A678" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="B678">
         <v>12</v>
@@ -81335,7 +81353,7 @@
     </row>
     <row r="679" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A679" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="B679">
         <v>13</v>
@@ -81454,7 +81472,7 @@
     </row>
     <row r="680" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A680" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="B680">
         <v>14</v>
@@ -81573,7 +81591,7 @@
     </row>
     <row r="681" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A681" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="B681">
         <v>15</v>
@@ -81692,7 +81710,7 @@
     </row>
     <row r="682" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A682" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="B682">
         <v>16</v>
@@ -81811,7 +81829,7 @@
     </row>
     <row r="683" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A683" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="B683">
         <v>17</v>
@@ -81930,7 +81948,7 @@
     </row>
     <row r="684" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A684" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="B684">
         <v>18</v>
@@ -82049,7 +82067,7 @@
     </row>
     <row r="685" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A685" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="B685">
         <v>19</v>
@@ -82168,7 +82186,7 @@
     </row>
     <row r="686" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A686" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="B686">
         <v>1</v>
@@ -82287,7 +82305,7 @@
     </row>
     <row r="687" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A687" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="B687">
         <v>2</v>
@@ -82406,7 +82424,7 @@
     </row>
     <row r="688" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A688" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="B688">
         <v>3</v>
@@ -82525,7 +82543,7 @@
     </row>
     <row r="689" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A689" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="B689">
         <v>4</v>
@@ -82644,7 +82662,7 @@
     </row>
     <row r="690" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A690" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="B690">
         <v>5</v>
@@ -82763,7 +82781,7 @@
     </row>
     <row r="691" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A691" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="B691">
         <v>6</v>
@@ -82882,7 +82900,7 @@
     </row>
     <row r="692" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A692" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="B692">
         <v>7</v>
@@ -83001,7 +83019,7 @@
     </row>
     <row r="693" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A693" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="B693">
         <v>8</v>
@@ -83120,7 +83138,7 @@
     </row>
     <row r="694" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A694" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="B694">
         <v>9</v>
@@ -83239,7 +83257,7 @@
     </row>
     <row r="695" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A695" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="B695">
         <v>10</v>
@@ -83358,7 +83376,7 @@
     </row>
     <row r="696" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A696" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="B696">
         <v>11</v>
@@ -83477,7 +83495,7 @@
     </row>
     <row r="697" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A697" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="B697">
         <v>12</v>
@@ -83596,7 +83614,7 @@
     </row>
     <row r="698" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A698" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="B698">
         <v>13</v>
@@ -83715,7 +83733,7 @@
     </row>
     <row r="699" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A699" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="B699">
         <v>14</v>
@@ -83834,7 +83852,7 @@
     </row>
     <row r="700" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A700" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="B700">
         <v>15</v>
@@ -83953,7 +83971,7 @@
     </row>
     <row r="701" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A701" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="B701">
         <v>16</v>
@@ -84072,7 +84090,7 @@
     </row>
     <row r="702" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A702" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="B702">
         <v>17</v>
@@ -84191,7 +84209,7 @@
     </row>
     <row r="703" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A703" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="B703">
         <v>18</v>
@@ -84310,7 +84328,7 @@
     </row>
     <row r="704" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A704" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="B704">
         <v>19</v>
@@ -84429,7 +84447,7 @@
     </row>
     <row r="705" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A705" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B705">
         <v>1</v>
@@ -84548,7 +84566,7 @@
     </row>
     <row r="706" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A706" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B706">
         <v>2</v>
@@ -84667,7 +84685,7 @@
     </row>
     <row r="707" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A707" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B707">
         <v>3</v>
@@ -84786,7 +84804,7 @@
     </row>
     <row r="708" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A708" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B708">
         <v>4</v>
@@ -84905,7 +84923,7 @@
     </row>
     <row r="709" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A709" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B709">
         <v>5</v>
@@ -85024,7 +85042,7 @@
     </row>
     <row r="710" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A710" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B710">
         <v>6</v>
@@ -85143,7 +85161,7 @@
     </row>
     <row r="711" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A711" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B711">
         <v>7</v>
@@ -85262,7 +85280,7 @@
     </row>
     <row r="712" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A712" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B712">
         <v>8</v>
@@ -85381,7 +85399,7 @@
     </row>
     <row r="713" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A713" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B713">
         <v>9</v>
@@ -85500,7 +85518,7 @@
     </row>
     <row r="714" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A714" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B714">
         <v>10</v>
@@ -85619,7 +85637,7 @@
     </row>
     <row r="715" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A715" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B715">
         <v>11</v>
@@ -85738,7 +85756,7 @@
     </row>
     <row r="716" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A716" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B716">
         <v>12</v>
@@ -85857,7 +85875,7 @@
     </row>
     <row r="717" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A717" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B717">
         <v>13</v>
@@ -85976,7 +85994,7 @@
     </row>
     <row r="718" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A718" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B718">
         <v>14</v>
@@ -86095,7 +86113,7 @@
     </row>
     <row r="719" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A719" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B719">
         <v>15</v>
@@ -86214,7 +86232,7 @@
     </row>
     <row r="720" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A720" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B720">
         <v>16</v>
@@ -86333,7 +86351,7 @@
     </row>
     <row r="721" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A721" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B721">
         <v>17</v>
@@ -86452,7 +86470,7 @@
     </row>
     <row r="722" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A722" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B722">
         <v>18</v>
@@ -86571,7 +86589,7 @@
     </row>
     <row r="723" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A723" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B723">
         <v>19</v>
@@ -86690,7 +86708,7 @@
     </row>
     <row r="724" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A724" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B724">
         <v>1</v>
@@ -86809,7 +86827,7 @@
     </row>
     <row r="725" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A725" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B725">
         <v>2</v>
@@ -86928,7 +86946,7 @@
     </row>
     <row r="726" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A726" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B726">
         <v>3</v>
@@ -87047,7 +87065,7 @@
     </row>
     <row r="727" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A727" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B727">
         <v>4</v>
@@ -87166,7 +87184,7 @@
     </row>
     <row r="728" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A728" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B728">
         <v>5</v>
@@ -87285,7 +87303,7 @@
     </row>
     <row r="729" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A729" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B729">
         <v>6</v>
@@ -87404,7 +87422,7 @@
     </row>
     <row r="730" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A730" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B730">
         <v>7</v>
@@ -87523,7 +87541,7 @@
     </row>
     <row r="731" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A731" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B731">
         <v>8</v>
@@ -87642,7 +87660,7 @@
     </row>
     <row r="732" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A732" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B732">
         <v>9</v>
@@ -87761,7 +87779,7 @@
     </row>
     <row r="733" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A733" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B733">
         <v>10</v>
@@ -87880,7 +87898,7 @@
     </row>
     <row r="734" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A734" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B734">
         <v>11</v>
@@ -87999,7 +88017,7 @@
     </row>
     <row r="735" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A735" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B735">
         <v>12</v>
@@ -88118,7 +88136,7 @@
     </row>
     <row r="736" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A736" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B736">
         <v>13</v>
@@ -88237,7 +88255,7 @@
     </row>
     <row r="737" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A737" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B737">
         <v>14</v>
@@ -88356,7 +88374,7 @@
     </row>
     <row r="738" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A738" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B738">
         <v>15</v>
@@ -88475,7 +88493,7 @@
     </row>
     <row r="739" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A739" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B739">
         <v>16</v>
@@ -88594,7 +88612,7 @@
     </row>
     <row r="740" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A740" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B740">
         <v>17</v>
@@ -88713,7 +88731,7 @@
     </row>
     <row r="741" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A741" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B741">
         <v>18</v>
@@ -88832,7 +88850,7 @@
     </row>
     <row r="742" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A742" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B742">
         <v>19</v>
@@ -88951,7 +88969,7 @@
     </row>
     <row r="743" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A743" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="B743">
         <v>1</v>
@@ -89070,7 +89088,7 @@
     </row>
     <row r="744" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A744" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="B744">
         <v>2</v>
@@ -89189,7 +89207,7 @@
     </row>
     <row r="745" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A745" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="B745">
         <v>3</v>
@@ -89308,7 +89326,7 @@
     </row>
     <row r="746" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A746" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="B746">
         <v>4</v>
@@ -89427,7 +89445,7 @@
     </row>
     <row r="747" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A747" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="B747">
         <v>5</v>
@@ -89546,7 +89564,7 @@
     </row>
     <row r="748" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A748" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="B748">
         <v>6</v>
@@ -89665,7 +89683,7 @@
     </row>
     <row r="749" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A749" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="B749">
         <v>7</v>
@@ -89784,7 +89802,7 @@
     </row>
     <row r="750" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A750" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="B750">
         <v>8</v>
@@ -89903,7 +89921,7 @@
     </row>
     <row r="751" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A751" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="B751">
         <v>9</v>
@@ -90022,7 +90040,7 @@
     </row>
     <row r="752" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A752" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="B752">
         <v>10</v>
@@ -90141,7 +90159,7 @@
     </row>
     <row r="753" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A753" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="B753">
         <v>11</v>
@@ -90260,7 +90278,7 @@
     </row>
     <row r="754" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A754" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="B754">
         <v>12</v>
@@ -90379,7 +90397,7 @@
     </row>
     <row r="755" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A755" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="B755">
         <v>13</v>
@@ -90498,7 +90516,7 @@
     </row>
     <row r="756" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A756" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="B756">
         <v>14</v>
@@ -90617,7 +90635,7 @@
     </row>
     <row r="757" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A757" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="B757">
         <v>15</v>
@@ -90736,7 +90754,7 @@
     </row>
     <row r="758" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A758" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="B758">
         <v>16</v>
@@ -90855,7 +90873,7 @@
     </row>
     <row r="759" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A759" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="B759">
         <v>17</v>
@@ -90974,7 +90992,7 @@
     </row>
     <row r="760" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A760" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="B760">
         <v>18</v>
@@ -91093,7 +91111,7 @@
     </row>
     <row r="761" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A761" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="B761">
         <v>19</v>
@@ -91212,7 +91230,7 @@
     </row>
     <row r="762" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A762" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="B762">
         <v>1</v>
@@ -91331,7 +91349,7 @@
     </row>
     <row r="763" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A763" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="B763">
         <v>2</v>
@@ -91450,7 +91468,7 @@
     </row>
     <row r="764" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A764" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="B764">
         <v>3</v>
@@ -91569,7 +91587,7 @@
     </row>
     <row r="765" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A765" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="B765">
         <v>4</v>
@@ -91688,7 +91706,7 @@
     </row>
     <row r="766" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A766" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="B766">
         <v>5</v>
@@ -91807,7 +91825,7 @@
     </row>
     <row r="767" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A767" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="B767">
         <v>6</v>
@@ -91926,7 +91944,7 @@
     </row>
     <row r="768" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A768" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="B768">
         <v>7</v>
@@ -92045,7 +92063,7 @@
     </row>
     <row r="769" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A769" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="B769">
         <v>8</v>
@@ -92164,7 +92182,7 @@
     </row>
     <row r="770" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A770" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="B770">
         <v>9</v>
@@ -92283,7 +92301,7 @@
     </row>
     <row r="771" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A771" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="B771">
         <v>10</v>
@@ -92402,7 +92420,7 @@
     </row>
     <row r="772" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A772" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="B772">
         <v>11</v>
@@ -92521,7 +92539,7 @@
     </row>
     <row r="773" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A773" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="B773">
         <v>12</v>
@@ -92640,7 +92658,7 @@
     </row>
     <row r="774" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A774" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="B774">
         <v>13</v>
@@ -92759,7 +92777,7 @@
     </row>
     <row r="775" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A775" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="B775">
         <v>14</v>
@@ -92878,7 +92896,7 @@
     </row>
     <row r="776" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A776" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="B776">
         <v>15</v>
@@ -92997,7 +93015,7 @@
     </row>
     <row r="777" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A777" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="B777">
         <v>16</v>
@@ -93116,7 +93134,7 @@
     </row>
     <row r="778" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A778" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="B778">
         <v>17</v>
@@ -93235,7 +93253,7 @@
     </row>
     <row r="779" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A779" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="B779">
         <v>18</v>
@@ -93354,7 +93372,7 @@
     </row>
     <row r="780" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A780" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="B780">
         <v>19</v>

</xml_diff>